<commit_message>
adding stochastic approximate inverse to siam talk
</commit_message>
<xml_diff>
--- a/doc/siam_cse_2015/data/siam_scaling.xlsx
+++ b/doc/siam_cse_2015/data/siam_scaling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="66360" yWindow="3100" windowWidth="25600" windowHeight="18400" tabRatio="500"/>
+    <workbookView xWindow="68380" yWindow="2120" windowWidth="20720" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>Communication Parameters</t>
   </si>
@@ -82,6 +82,48 @@
   </si>
   <si>
     <t>Strong Scaling</t>
+  </si>
+  <si>
+    <t>Replication Scaling</t>
+  </si>
+  <si>
+    <t>Sets</t>
+  </si>
+  <si>
+    <t>Performance Comparison</t>
+  </si>
+  <si>
+    <t>Belos GMRES</t>
+  </si>
+  <si>
+    <t>MCLS MCSA</t>
+  </si>
+  <si>
+    <t>Temere MCSA</t>
+  </si>
+  <si>
+    <t>Iters</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Strong Scaling Test Details</t>
+  </si>
+  <si>
+    <t>Replication Scaling Test Details</t>
+  </si>
+  <si>
+    <t>Performance Comparison Test Details</t>
+  </si>
+  <si>
+    <t>Tolerance</t>
+  </si>
+  <si>
+    <t>Scaling</t>
+  </si>
+  <si>
+    <t>Block Jacobi</t>
   </si>
 </sst>
 </file>
@@ -255,7 +297,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -297,8 +339,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -334,8 +412,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -356,6 +437,24 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -376,6 +475,24 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -705,15 +822,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N42"/>
+  <dimension ref="A2:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="10" max="11" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1432,7 +1551,7 @@
         <v>19</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="N37" s="16"/>
     </row>
@@ -1583,6 +1702,273 @@
       <c r="I42" s="28" t="e">
         <f t="shared" si="14"/>
         <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="6">
+        <v>1</v>
+      </c>
+      <c r="B47" s="7">
+        <v>256</v>
+      </c>
+      <c r="C47" s="7">
+        <f>B47/16</f>
+        <v>16</v>
+      </c>
+      <c r="D47" s="33">
+        <v>6473600</v>
+      </c>
+      <c r="E47" s="33">
+        <f>D47/B47</f>
+        <v>25287.5</v>
+      </c>
+      <c r="F47" s="7">
+        <v>6.4928999999999997</v>
+      </c>
+      <c r="G47" s="7">
+        <v>6.4931000000000001</v>
+      </c>
+      <c r="H47" s="7">
+        <v>6.4930000000000003</v>
+      </c>
+      <c r="I47" s="9">
+        <f>G47*A47/$G$47</f>
+        <v>1</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="6">
+        <v>2</v>
+      </c>
+      <c r="B48" s="7">
+        <f>$B$47*A48</f>
+        <v>512</v>
+      </c>
+      <c r="C48" s="7">
+        <f t="shared" ref="C48:C50" si="15">B48/16</f>
+        <v>32</v>
+      </c>
+      <c r="D48" s="33">
+        <v>6473600</v>
+      </c>
+      <c r="E48" s="33">
+        <f>E47</f>
+        <v>25287.5</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="9">
+        <f t="shared" ref="I48:I50" si="16">G48*A48/$G$47</f>
+        <v>0</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="6">
+        <v>3</v>
+      </c>
+      <c r="B49" s="7">
+        <f t="shared" ref="B49:B50" si="17">$B$47*A49</f>
+        <v>768</v>
+      </c>
+      <c r="C49" s="7">
+        <f t="shared" si="15"/>
+        <v>48</v>
+      </c>
+      <c r="D49" s="33">
+        <v>6473600</v>
+      </c>
+      <c r="E49" s="33">
+        <f>E48</f>
+        <v>25287.5</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="9">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="13">
+        <v>4</v>
+      </c>
+      <c r="B50" s="14">
+        <f t="shared" si="17"/>
+        <v>1024</v>
+      </c>
+      <c r="C50" s="14">
+        <f t="shared" si="15"/>
+        <v>64</v>
+      </c>
+      <c r="D50" s="34">
+        <v>6473600</v>
+      </c>
+      <c r="E50" s="34">
+        <f>E49</f>
+        <v>25287.5</v>
+      </c>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="15">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="6"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="9"/>
+      <c r="K54" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="6"/>
+      <c r="B55" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" s="7"/>
+      <c r="C56" s="9"/>
+      <c r="K56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L56">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="7"/>
+      <c r="C57" s="9"/>
+      <c r="K57" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L57" s="36">
+        <v>1E-8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="14"/>
+      <c r="C58" s="15"/>
+      <c r="K58" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="K60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N60" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="K61">
+        <v>64</v>
+      </c>
+      <c r="L61">
+        <v>4</v>
+      </c>
+      <c r="M61">
+        <v>1618400</v>
+      </c>
+      <c r="N61">
+        <v>25287.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding more data to siam talk
</commit_message>
<xml_diff>
--- a/doc/siam_cse_2015/data/siam_scaling.xlsx
+++ b/doc/siam_cse_2015/data/siam_scaling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="68380" yWindow="2120" windowWidth="20720" windowHeight="24000" tabRatio="500"/>
+    <workbookView xWindow="69540" yWindow="2120" windowWidth="19940" windowHeight="24000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -825,7 +825,7 @@
   <dimension ref="A2:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1607,10 +1607,12 @@
         <f t="shared" si="12"/>
         <v>64</v>
       </c>
-      <c r="D39" s="33"/>
+      <c r="D39" s="33">
+        <v>273509600</v>
+      </c>
       <c r="E39" s="33">
         <f t="shared" ref="E39:E42" si="13">D39/B39</f>
-        <v>0</v>
+        <v>267099.21875</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
@@ -1639,10 +1641,12 @@
         <f t="shared" si="12"/>
         <v>256</v>
       </c>
-      <c r="D40" s="33"/>
+      <c r="D40" s="33">
+        <v>273509600</v>
+      </c>
       <c r="E40" s="33">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>66774.8046875</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
@@ -1665,10 +1669,12 @@
         <f t="shared" si="12"/>
         <v>484</v>
       </c>
-      <c r="D41" s="33"/>
+      <c r="D41" s="33">
+        <v>273509600</v>
+      </c>
       <c r="E41" s="33">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>35318.904958677689</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -1691,10 +1697,12 @@
         <f t="shared" si="12"/>
         <v>676</v>
       </c>
-      <c r="D42" s="34"/>
+      <c r="D42" s="33">
+        <v>273509600</v>
+      </c>
       <c r="E42" s="34">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>25287.5</v>
       </c>
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>

</xml_diff>

<commit_message>
updating strong scaling data and loop figure for siam talk
</commit_message>
<xml_diff>
--- a/doc/siam_cse_2015/data/siam_scaling.xlsx
+++ b/doc/siam_cse_2015/data/siam_scaling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="69540" yWindow="2120" windowWidth="19940" windowHeight="24000" tabRatio="500"/>
+    <workbookView xWindow="21640" yWindow="0" windowWidth="21320" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -825,7 +825,7 @@
   <dimension ref="A2:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1584,7 +1584,7 @@
         <v>260.54000000000002</v>
       </c>
       <c r="I38" s="26">
-        <f>($G$38/$B$38)/(G38/B38)</f>
+        <f>($G$38*$B$38)/(G38*B38)</f>
         <v>1</v>
       </c>
       <c r="K38" s="2" t="s">
@@ -1614,12 +1614,18 @@
         <f t="shared" ref="E39:E42" si="13">D39/B39</f>
         <v>267099.21875</v>
       </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="26" t="e">
-        <f t="shared" ref="I39:I42" si="14">($G$38/$B$38)/(G39/B39)</f>
-        <v>#DIV/0!</v>
+      <c r="F39" s="7">
+        <v>61.918999999999997</v>
+      </c>
+      <c r="G39" s="7">
+        <v>61.920999999999999</v>
+      </c>
+      <c r="H39" s="7">
+        <v>61.92</v>
+      </c>
+      <c r="I39" s="26">
+        <f t="shared" ref="I39:I42" si="14">($G$38*$B$38)/(G39*B39)</f>
+        <v>1.0519048464979572</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>8</v>
@@ -1697,7 +1703,7 @@
         <f t="shared" si="12"/>
         <v>676</v>
       </c>
-      <c r="D42" s="33">
+      <c r="D42" s="34">
         <v>273509600</v>
       </c>
       <c r="E42" s="34">

</xml_diff>

<commit_message>
adding titan scaling data
</commit_message>
<xml_diff>
--- a/doc/siam_cse_2015/data/siam_scaling.xlsx
+++ b/doc/siam_cse_2015/data/siam_scaling.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="21640" yWindow="0" windowWidth="21320" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="15700" yWindow="0" windowWidth="12860" windowHeight="17640" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="titan" sheetId="2" r:id="rId1"/>
+    <sheet name="eos" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="35">
   <si>
     <t>Communication Parameters</t>
   </si>
@@ -297,7 +298,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -375,8 +376,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -415,8 +426,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -455,6 +479,11 @@
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -493,6 +522,11 @@
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -824,7 +858,1137 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="10" max="11" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="K2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="K3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="10">
+        <v>128</v>
+      </c>
+      <c r="D4" s="10">
+        <v>256</v>
+      </c>
+      <c r="E4" s="10">
+        <v>512</v>
+      </c>
+      <c r="F4" s="11">
+        <v>1024</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="K4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="6"/>
+      <c r="B5" s="10">
+        <v>256</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="K5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="6"/>
+      <c r="B6" s="10">
+        <v>512</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="K6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="16">
+        <v>1618400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1024</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="K7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="16">
+        <f>L6/L3</f>
+        <v>25287.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="6"/>
+      <c r="B8" s="10">
+        <v>2048</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="K8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="6"/>
+      <c r="B9" s="10">
+        <v>4096</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="K9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="6"/>
+      <c r="B10" s="17">
+        <v>8192</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="13"/>
+      <c r="B11" s="24">
+        <v>16384</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="10">
+        <v>128</v>
+      </c>
+      <c r="D15" s="10">
+        <v>256</v>
+      </c>
+      <c r="E15" s="10">
+        <v>512</v>
+      </c>
+      <c r="F15" s="11">
+        <v>1024</v>
+      </c>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="6"/>
+      <c r="B16" s="10">
+        <v>256</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="6"/>
+      <c r="B17" s="10">
+        <v>512</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="10">
+        <v>1024</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="6"/>
+      <c r="B19" s="10">
+        <v>2048</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="6"/>
+      <c r="B20" s="10">
+        <v>4096</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="6"/>
+      <c r="B21" s="17">
+        <v>8192</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="13"/>
+      <c r="B22" s="24">
+        <v>16384</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="6">
+        <v>1</v>
+      </c>
+      <c r="B28" s="33">
+        <f>64*A28*A28</f>
+        <v>64</v>
+      </c>
+      <c r="C28" s="33">
+        <f>B28/16</f>
+        <v>4</v>
+      </c>
+      <c r="D28" s="33">
+        <v>1618400</v>
+      </c>
+      <c r="E28" s="33">
+        <f>D28/B28</f>
+        <v>25287.5</v>
+      </c>
+      <c r="F28" s="25">
+        <v>12.648</v>
+      </c>
+      <c r="G28" s="25">
+        <v>12.648</v>
+      </c>
+      <c r="H28" s="25">
+        <v>12.648</v>
+      </c>
+      <c r="I28" s="26">
+        <f>$G$28/G28</f>
+        <v>1</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="6">
+        <v>2</v>
+      </c>
+      <c r="B29" s="33">
+        <f t="shared" ref="B29:B30" si="0">64*A29*A29</f>
+        <v>256</v>
+      </c>
+      <c r="C29" s="33">
+        <f t="shared" ref="C29:C33" si="1">B29/16</f>
+        <v>16</v>
+      </c>
+      <c r="D29" s="33">
+        <v>6473600</v>
+      </c>
+      <c r="E29" s="33">
+        <f t="shared" ref="E29:E33" si="2">D29/B29</f>
+        <v>25287.5</v>
+      </c>
+      <c r="F29" s="25">
+        <v>12.86</v>
+      </c>
+      <c r="G29" s="25">
+        <v>12.861000000000001</v>
+      </c>
+      <c r="H29" s="25">
+        <v>12.861000000000001</v>
+      </c>
+      <c r="I29" s="26">
+        <f t="shared" ref="I29:I33" si="3">$G$28/G29</f>
+        <v>0.98343830184278047</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="6">
+        <v>4</v>
+      </c>
+      <c r="B30" s="33">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+      <c r="C30" s="33">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="D30" s="33">
+        <v>25894400</v>
+      </c>
+      <c r="E30" s="33">
+        <f t="shared" si="2"/>
+        <v>25287.5</v>
+      </c>
+      <c r="F30" s="25">
+        <v>14.587999999999999</v>
+      </c>
+      <c r="G30" s="25">
+        <v>14.589</v>
+      </c>
+      <c r="H30" s="25">
+        <v>14.589</v>
+      </c>
+      <c r="I30" s="26">
+        <f t="shared" si="3"/>
+        <v>0.8669545548015628</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="6">
+        <v>8</v>
+      </c>
+      <c r="B31" s="33">
+        <f>64*A31*A31</f>
+        <v>4096</v>
+      </c>
+      <c r="C31" s="33">
+        <f t="shared" si="1"/>
+        <v>256</v>
+      </c>
+      <c r="D31" s="33">
+        <v>103577600</v>
+      </c>
+      <c r="E31" s="33">
+        <f t="shared" si="2"/>
+        <v>25287.5</v>
+      </c>
+      <c r="F31" s="25">
+        <v>14.252000000000001</v>
+      </c>
+      <c r="G31" s="25">
+        <v>14.253</v>
+      </c>
+      <c r="H31" s="25">
+        <v>14.253</v>
+      </c>
+      <c r="I31" s="26">
+        <f t="shared" si="3"/>
+        <v>0.88739212797305822</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="6">
+        <v>11</v>
+      </c>
+      <c r="B32" s="33">
+        <f>64*A32*A32</f>
+        <v>7744</v>
+      </c>
+      <c r="C32" s="33">
+        <f t="shared" si="1"/>
+        <v>484</v>
+      </c>
+      <c r="D32" s="33">
+        <v>195826400</v>
+      </c>
+      <c r="E32" s="33">
+        <f t="shared" si="2"/>
+        <v>25287.5</v>
+      </c>
+      <c r="F32" s="25">
+        <v>14.747</v>
+      </c>
+      <c r="G32" s="25">
+        <v>14.778</v>
+      </c>
+      <c r="H32" s="25">
+        <v>14.747</v>
+      </c>
+      <c r="I32" s="26">
+        <f t="shared" si="3"/>
+        <v>0.85586682907023948</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="13">
+        <v>13</v>
+      </c>
+      <c r="B33" s="34">
+        <f>64*A33*A33</f>
+        <v>10816</v>
+      </c>
+      <c r="C33" s="34">
+        <f t="shared" si="1"/>
+        <v>676</v>
+      </c>
+      <c r="D33" s="34">
+        <v>273509600</v>
+      </c>
+      <c r="E33" s="34">
+        <f t="shared" si="2"/>
+        <v>25287.5</v>
+      </c>
+      <c r="F33" s="27">
+        <v>13.721</v>
+      </c>
+      <c r="G33" s="27">
+        <v>13.724</v>
+      </c>
+      <c r="H33" s="27">
+        <v>13.723000000000001</v>
+      </c>
+      <c r="I33" s="28">
+        <f t="shared" si="3"/>
+        <v>0.9215972019819294</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="N35" s="16"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="5"/>
+      <c r="N36" s="16"/>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N37" s="16"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="6">
+        <v>2</v>
+      </c>
+      <c r="B38" s="33">
+        <f t="shared" ref="B38:B39" si="4">64*A38*A38</f>
+        <v>256</v>
+      </c>
+      <c r="C38" s="33">
+        <f t="shared" ref="C38:C42" si="5">B38/16</f>
+        <v>16</v>
+      </c>
+      <c r="D38" s="33">
+        <v>273509600</v>
+      </c>
+      <c r="E38" s="33">
+        <f>D38/B38</f>
+        <v>1068396.875</v>
+      </c>
+      <c r="F38" s="25">
+        <v>515.51</v>
+      </c>
+      <c r="G38" s="25">
+        <v>515.52</v>
+      </c>
+      <c r="H38" s="25">
+        <v>515.52</v>
+      </c>
+      <c r="I38" s="26">
+        <f>($G$38*$B$38)/(G38*B38)</f>
+        <v>1</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L38">
+        <v>3</v>
+      </c>
+      <c r="N38" s="16"/>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="6">
+        <v>4</v>
+      </c>
+      <c r="B39" s="33">
+        <f t="shared" si="4"/>
+        <v>1024</v>
+      </c>
+      <c r="C39" s="33">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="D39" s="33">
+        <v>273509600</v>
+      </c>
+      <c r="E39" s="33">
+        <f t="shared" ref="E39:E42" si="6">D39/B39</f>
+        <v>267099.21875</v>
+      </c>
+      <c r="F39" s="25">
+        <v>122.76</v>
+      </c>
+      <c r="G39" s="25">
+        <v>122.77</v>
+      </c>
+      <c r="H39" s="25">
+        <v>122.76</v>
+      </c>
+      <c r="I39" s="26">
+        <f t="shared" ref="I39:I42" si="7">($G$38*$B$38)/(G39*B39)</f>
+        <v>1.0497678585973773</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L39">
+        <v>15</v>
+      </c>
+      <c r="N39" s="16"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="6">
+        <v>8</v>
+      </c>
+      <c r="B40" s="33">
+        <f>64*A40*A40</f>
+        <v>4096</v>
+      </c>
+      <c r="C40" s="33">
+        <f t="shared" si="5"/>
+        <v>256</v>
+      </c>
+      <c r="D40" s="33">
+        <v>273509600</v>
+      </c>
+      <c r="E40" s="33">
+        <f t="shared" si="6"/>
+        <v>66774.8046875</v>
+      </c>
+      <c r="F40" s="25">
+        <v>27.963000000000001</v>
+      </c>
+      <c r="G40" s="25">
+        <v>27.966000000000001</v>
+      </c>
+      <c r="H40" s="25">
+        <v>27.963999999999999</v>
+      </c>
+      <c r="I40" s="26">
+        <f t="shared" si="7"/>
+        <v>1.1521132804119287</v>
+      </c>
+      <c r="N40" s="16"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="6">
+        <v>11</v>
+      </c>
+      <c r="B41" s="33">
+        <f>64*A41*A41</f>
+        <v>7744</v>
+      </c>
+      <c r="C41" s="33">
+        <f t="shared" si="5"/>
+        <v>484</v>
+      </c>
+      <c r="D41" s="33">
+        <v>273509600</v>
+      </c>
+      <c r="E41" s="33">
+        <f t="shared" si="6"/>
+        <v>35318.904958677689</v>
+      </c>
+      <c r="F41" s="25">
+        <v>17.715</v>
+      </c>
+      <c r="G41" s="25">
+        <v>17.716000000000001</v>
+      </c>
+      <c r="H41" s="25">
+        <v>17.715</v>
+      </c>
+      <c r="I41" s="26">
+        <f t="shared" si="7"/>
+        <v>0.96195436165468384</v>
+      </c>
+      <c r="N41" s="16"/>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="13">
+        <v>13</v>
+      </c>
+      <c r="B42" s="34">
+        <f>64*A42*A42</f>
+        <v>10816</v>
+      </c>
+      <c r="C42" s="34">
+        <f t="shared" si="5"/>
+        <v>676</v>
+      </c>
+      <c r="D42" s="34">
+        <v>273509600</v>
+      </c>
+      <c r="E42" s="34">
+        <f t="shared" si="6"/>
+        <v>25287.5</v>
+      </c>
+      <c r="F42" s="27">
+        <v>13.72</v>
+      </c>
+      <c r="G42" s="27">
+        <v>13.721</v>
+      </c>
+      <c r="H42" s="27">
+        <v>13.721</v>
+      </c>
+      <c r="I42" s="28">
+        <f t="shared" si="7"/>
+        <v>0.88926877084277578</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="42"/>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="43"/>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="H46" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="47">
+        <v>1</v>
+      </c>
+      <c r="B47" s="48">
+        <v>256</v>
+      </c>
+      <c r="C47" s="48">
+        <f>B47/16</f>
+        <v>16</v>
+      </c>
+      <c r="D47" s="48">
+        <v>6473600</v>
+      </c>
+      <c r="E47" s="48">
+        <f>D47/B47</f>
+        <v>25287.5</v>
+      </c>
+      <c r="F47" s="48">
+        <f>12.648+0.001399</f>
+        <v>12.649398999999999</v>
+      </c>
+      <c r="G47" s="48">
+        <v>12.648999999999999</v>
+      </c>
+      <c r="H47" s="48">
+        <v>12.648999999999999</v>
+      </c>
+      <c r="I47" s="26">
+        <f>$G$47/(G47*A47)</f>
+        <v>1</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="47">
+        <v>2</v>
+      </c>
+      <c r="B48" s="48">
+        <f>$B$47*A48</f>
+        <v>512</v>
+      </c>
+      <c r="C48" s="48">
+        <f t="shared" ref="C48:C50" si="8">B48/16</f>
+        <v>32</v>
+      </c>
+      <c r="D48" s="48">
+        <v>6473600</v>
+      </c>
+      <c r="E48" s="48">
+        <f>E47</f>
+        <v>25287.5</v>
+      </c>
+      <c r="F48" s="48">
+        <f>0.014895+6.6051</f>
+        <v>6.6199950000000003</v>
+      </c>
+      <c r="G48" s="48">
+        <f>0.17423+6.6286</f>
+        <v>6.8028299999999993</v>
+      </c>
+      <c r="H48" s="48">
+        <f>6.6168+0.10218</f>
+        <v>6.7189799999999993</v>
+      </c>
+      <c r="I48" s="26">
+        <f t="shared" ref="I48:I50" si="9">$G$47/(G48*A48)</f>
+        <v>0.92968661571728239</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="47">
+        <v>3</v>
+      </c>
+      <c r="B49" s="48">
+        <f t="shared" ref="B49:B50" si="10">$B$47*A49</f>
+        <v>768</v>
+      </c>
+      <c r="C49" s="48">
+        <f t="shared" si="8"/>
+        <v>48</v>
+      </c>
+      <c r="D49" s="48">
+        <v>6473600</v>
+      </c>
+      <c r="E49" s="48">
+        <f>E48</f>
+        <v>25287.5</v>
+      </c>
+      <c r="F49" s="48">
+        <f>0.035887+4.5638</f>
+        <v>4.5996869999999994</v>
+      </c>
+      <c r="G49" s="48">
+        <f>4.6158+0.11854</f>
+        <v>4.7343400000000004</v>
+      </c>
+      <c r="H49" s="48">
+        <f>0.068709+4.5952</f>
+        <v>4.6639090000000003</v>
+      </c>
+      <c r="I49" s="26">
+        <f t="shared" si="9"/>
+        <v>0.89058524173027975</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="49">
+        <v>4</v>
+      </c>
+      <c r="B50" s="50">
+        <f t="shared" si="10"/>
+        <v>1024</v>
+      </c>
+      <c r="C50" s="50">
+        <f t="shared" si="8"/>
+        <v>64</v>
+      </c>
+      <c r="D50" s="50">
+        <v>6473600</v>
+      </c>
+      <c r="E50" s="50">
+        <f>E49</f>
+        <v>25287.5</v>
+      </c>
+      <c r="F50" s="50">
+        <f>0.078491+3.5427</f>
+        <v>3.621191</v>
+      </c>
+      <c r="G50" s="50">
+        <f>3.5852+0.22359</f>
+        <v>3.8087900000000001</v>
+      </c>
+      <c r="H50" s="50">
+        <f>3.5667+0.1467</f>
+        <v>3.7134</v>
+      </c>
+      <c r="I50" s="28">
+        <f t="shared" si="9"/>
+        <v>0.83025055201258136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="6"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="9"/>
+      <c r="K54" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="6"/>
+      <c r="B55" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" s="7"/>
+      <c r="C56" s="9"/>
+      <c r="K56" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L56">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14">
+      <c r="A57" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="7"/>
+      <c r="C57" s="9"/>
+      <c r="K57" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L57" s="36">
+        <v>1E-8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14">
+      <c r="A58" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" s="14"/>
+      <c r="C58" s="15"/>
+      <c r="K58" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14">
+      <c r="K60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M60" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N60" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14">
+      <c r="K61">
+        <v>64</v>
+      </c>
+      <c r="L61">
+        <v>4</v>
+      </c>
+      <c r="M61">
+        <v>1618400</v>
+      </c>
+      <c r="N61">
+        <v>25287.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding titan data to siam talk
</commit_message>
<xml_diff>
--- a/doc/siam_cse_2015/data/siam_scaling.xlsx
+++ b/doc/siam_cse_2015/data/siam_scaling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15700" yWindow="0" windowWidth="12860" windowHeight="17640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="titan" sheetId="2" r:id="rId1"/>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
working on reviewer comments
</commit_message>
<xml_diff>
--- a/doc/siam_cse_2015/data/siam_scaling.xlsx
+++ b/doc/siam_cse_2015/data/siam_scaling.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="50">
   <si>
     <t>Communication Parameters</t>
   </si>
@@ -125,6 +125,51 @@
   </si>
   <si>
     <t>Block Jacobi</t>
+  </si>
+  <si>
+    <t>Replication 4 sets</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Set-AllReduce</t>
+  </si>
+  <si>
+    <t>Set-AllToAll</t>
+  </si>
+  <si>
+    <t>Block-AllReduce</t>
+  </si>
+  <si>
+    <t>Block-AllToAll</t>
+  </si>
+  <si>
+    <t>MC Min</t>
+  </si>
+  <si>
+    <t>MC Ave</t>
+  </si>
+  <si>
+    <t>MC Max</t>
+  </si>
+  <si>
+    <t>Sum Min</t>
+  </si>
+  <si>
+    <t>Sum Max</t>
+  </si>
+  <si>
+    <t>Sum Ave</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Ave</t>
+  </si>
+  <si>
+    <t>Max</t>
   </si>
 </sst>
 </file>
@@ -298,7 +343,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -386,8 +431,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -439,8 +508,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -484,6 +559,18 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -527,6 +614,18 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -856,15 +955,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N61"/>
+  <dimension ref="A2:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="10" max="11" width="13.5" customWidth="1"/>
@@ -1972,6 +2071,150 @@
       <c r="N61">
         <v>25287.5</v>
       </c>
+    </row>
+    <row r="64" spans="1:14">
+      <c r="A64" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="B65" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="E65" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="G65" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="H65" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="I65" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="J65" s="51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B66" s="52">
+        <v>3.5470000000000002</v>
+      </c>
+      <c r="C66" s="52">
+        <v>3.5653999999999999</v>
+      </c>
+      <c r="D66" s="52">
+        <v>3.5842999999999998</v>
+      </c>
+      <c r="E66" s="52">
+        <v>4.1291000000000001E-2</v>
+      </c>
+      <c r="F66" s="52">
+        <v>0.13708000000000001</v>
+      </c>
+      <c r="G66" s="52">
+        <v>0.19917000000000001</v>
+      </c>
+      <c r="H66" s="52">
+        <f>B66+E66</f>
+        <v>3.5882910000000003</v>
+      </c>
+      <c r="I66" s="52">
+        <f>C66+F66</f>
+        <v>3.70248</v>
+      </c>
+      <c r="J66" s="52">
+        <f>D66+G66</f>
+        <v>3.7834699999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="B67" s="52">
+        <v>3.7547999999999999</v>
+      </c>
+      <c r="C67" s="52">
+        <v>3.7799</v>
+      </c>
+      <c r="D67" s="52">
+        <v>3.8121</v>
+      </c>
+      <c r="E67" s="52">
+        <v>3.1574999999999999E-2</v>
+      </c>
+      <c r="F67" s="52">
+        <v>8.8168999999999997E-2</v>
+      </c>
+      <c r="G67" s="52">
+        <v>0.15418999999999999</v>
+      </c>
+      <c r="H67" s="52">
+        <f t="shared" ref="H67:H69" si="11">B67+E67</f>
+        <v>3.786375</v>
+      </c>
+      <c r="I67" s="52">
+        <f t="shared" ref="I67:I69" si="12">C67+F67</f>
+        <v>3.8680690000000002</v>
+      </c>
+      <c r="J67" s="52">
+        <f t="shared" ref="J67:J69" si="13">D67+G67</f>
+        <v>3.9662899999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>